<commit_message>
DE PARA CAMPOS STG ODS_IES
</commit_message>
<xml_diff>
--- a/modelagem/dicionário_dados_educação_superior.xlsx
+++ b/modelagem/dicionário_dados_educação_superior.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\analise-dados-evasao\modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54DC357-1D70-4E79-985D-A1D7D704C57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424B8296-30D1-4EEA-85F6-0B6F86854AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastro_cursos_wrk" sheetId="6" r:id="rId1"/>
     <sheet name="cadastro_ies_wrk" sheetId="5" r:id="rId2"/>
     <sheet name="cadastro_cursos" sheetId="4" r:id="rId3"/>
     <sheet name="cadastro_ies" sheetId="2" r:id="rId4"/>
+    <sheet name="DINAMICA_DE_PARA IES" sheetId="8" r:id="rId5"/>
+    <sheet name="DADOS_DE_PARA_STG_ODS_IES" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">cadastro_cursos!$A$8:$U$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cadastro_cursos_wrk!$A$1:$V$202</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">cadastro_ies!$A$8:$U$85</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cadastro_ies_wrk!$A$1:$U$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">DADOS_DE_PARA_STG_ODS_IES!$A$1:$B$46</definedName>
     <definedName name="Ies">#REF!</definedName>
     <definedName name="les_n">#REF!</definedName>
     <definedName name="lesles">#REF!</definedName>
@@ -30,6 +33,9 @@
     <definedName name="sit_n">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="15" r:id="rId7"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -46,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9290" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9466" uniqueCount="660">
   <si>
     <t>Alteração de nomenclatura</t>
   </si>
@@ -1927,16 +1933,158 @@
   <si>
     <t>Usar?</t>
   </si>
+  <si>
+    <t>Total Geral</t>
+  </si>
+  <si>
+    <t>VL_IGC</t>
+  </si>
+  <si>
+    <t>VL_CI_EAD</t>
+  </si>
+  <si>
+    <t>NU_CI</t>
+  </si>
+  <si>
+    <t>NU_CEP</t>
+  </si>
+  <si>
+    <t>NU_ANO_IGC</t>
+  </si>
+  <si>
+    <t>NU_ANO_CI_EAD</t>
+  </si>
+  <si>
+    <t>NU_ANO_CI</t>
+  </si>
+  <si>
+    <t>NO_TIPO_CREDENCIAMENTO</t>
+  </si>
+  <si>
+    <t>LEVAR PARA ODS</t>
+  </si>
+  <si>
+    <t>NO_SITUACAO_IES</t>
+  </si>
+  <si>
+    <t>NÃO LEVAR PARA ODS</t>
+  </si>
+  <si>
+    <t>NO_REDE</t>
+  </si>
+  <si>
+    <t>NO_ORGANIZACAO_ACADEMICA</t>
+  </si>
+  <si>
+    <t>NO_NATUREZA_JURIDICA</t>
+  </si>
+  <si>
+    <t>NO_CATEGORIA_ADMINISTRATIVA</t>
+  </si>
+  <si>
+    <t>DEIXAR NULO</t>
+  </si>
+  <si>
+    <t>NO_BAIRRO</t>
+  </si>
+  <si>
+    <t>DEIXAR NULO; VERIFICAR COMO CARREGAR CAMPO</t>
+  </si>
+  <si>
+    <t>DT_CRIACAO</t>
+  </si>
+  <si>
+    <t>DS_TELEFONE</t>
+  </si>
+  <si>
+    <t>DS_SITE</t>
+  </si>
+  <si>
+    <t>DS_SINALIZACAO_VIGENTE</t>
+  </si>
+  <si>
+    <t>DS_REPRESENTANTE_LEGAL</t>
+  </si>
+  <si>
+    <t>DS_REITOR_PRINCIPAL</t>
+  </si>
+  <si>
+    <t>DS_NUMERO_ENDERECO</t>
+  </si>
+  <si>
+    <t>DS_ENDERECO</t>
+  </si>
+  <si>
+    <t>DS_EMAIL</t>
+  </si>
+  <si>
+    <t>REMOVER DA ODS</t>
+  </si>
+  <si>
+    <t>DS_COMPLEMENTO_ENDERECO</t>
+  </si>
+  <si>
+    <t>CO_CNPJ</t>
+  </si>
+  <si>
+    <t>STG_IES</t>
+  </si>
+  <si>
+    <t>ODS_IES</t>
+  </si>
+  <si>
+    <t>Rótulos de Linha</t>
+  </si>
+  <si>
+    <t>Rótulos de Coluna</t>
+  </si>
+  <si>
+    <t>Contagem de COLUNA</t>
+  </si>
+  <si>
+    <t>TABELA</t>
+  </si>
+  <si>
+    <t>COLUNA</t>
+  </si>
+  <si>
+    <t>OK; LEVAR PARA ODS</t>
+  </si>
+  <si>
+    <t>NÃO TEM NA TABELA; NECESSARIO FAZER JOIN PELO NOME DO MUNICIPIO PARA OBTER O CÓDIGO E LEVAR PARA ODS</t>
+  </si>
+  <si>
+    <t>NÃO TEM NA TABELA; CARREGAR VIA CASE (UTILIZAR DICIONARIO DE DADOS DA COLUNA)</t>
+  </si>
+  <si>
+    <t>"NÃO TEM NA TABELA; NECESSARIO FAZER JOIN PELO NOME DO MUNICIPIO PARA OBTER O CÓDIGO E LEVAR PARA ODS; 
+EXEMPLO
+CASE 
+	WHEN ies.NO_REDE = 'Publica' then 1 
+	WHEN ies.NO_REDE = 'Privada' then 2
+	ELSE 0 
+END TP_REDE	"</t>
+  </si>
+  <si>
+    <t>TAREFA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2047,7 +2195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2100,6 +2248,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFC5E0B3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2253,312 +2407,313 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="3" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2567,89 +2722,98 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="8" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="8" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="8" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="8"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="8" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="8" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="8" pivotButton="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="8" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{3EB83FEC-FF46-4DAF-B9B3-569CB6A01E40}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{4A332866-B4F8-4F30-A262-866BAC8C4646}"/>
@@ -2658,8 +2822,59 @@
     <cellStyle name="Normal 4 2" xfId="4" xr:uid="{979B69FA-E084-4FBE-AC84-9439175AF9AD}"/>
     <cellStyle name="Normal 5" xfId="6" xr:uid="{20F855B5-7D00-4791-B6C2-B95DEB859FC2}"/>
     <cellStyle name="Normal 6" xfId="7" xr:uid="{2A3A651F-1AC2-48B7-9FD8-795CF8989298}"/>
+    <cellStyle name="Normal 7" xfId="8" xr:uid="{C7F240D9-118F-4F9A-A643-81827ECFAFE3}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2670,6 +2885,586 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="admin" refreshedDate="45199.871260648149" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="45" xr:uid="{52B1D66E-9DF3-4FE1-9082-E4EAD6E8EF86}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:B46" sheet="Planilha1 (2)" r:id="rId2"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="COLUNA" numFmtId="0">
+      <sharedItems count="44">
+        <s v="CO_IES"/>
+        <s v="NO_IES"/>
+        <s v="SG_IES"/>
+        <s v="NU_ANO_CENSO"/>
+        <s v="CO_MUNICIPIO"/>
+        <s v="IN_CAPITAL"/>
+        <s v="TP_ORGANIZACAO_ACADEMICA"/>
+        <s v="TP_CATEGORIA_ADMINISTRATIVA"/>
+        <s v="CO_MANTENEDORA"/>
+        <s v="DS_ENDERECO"/>
+        <s v="DS_NUMERO_ENDERECO"/>
+        <s v="DS_COMPLEMENTO_ENDERECO"/>
+        <s v="NO_BAIRRO"/>
+        <s v="NU_CEP"/>
+        <s v="NO_CATEGORIA_ADMINISTRATIVA"/>
+        <s v="NO_ORGANIZACAO_ACADEMICA"/>
+        <s v="TP_REDE"/>
+        <s v="NO_MANTENEDORA"/>
+        <s v="CO_CNPJ"/>
+        <s v="NO_NATUREZA_JURIDICA"/>
+        <s v="DS_TELEFONE"/>
+        <s v="DS_SITE"/>
+        <s v="DS_EMAIL"/>
+        <s v="NO_MUNICIPIO"/>
+        <s v="SG_UF"/>
+        <s v="NO_TIPO_CREDENCIAMENTO"/>
+        <s v="NO_REDE"/>
+        <s v="DT_CRIACAO"/>
+        <s v="NU_CI"/>
+        <s v="NU_ANO_CI"/>
+        <s v="VL_CI_EAD"/>
+        <s v="NU_ANO_CI_EAD"/>
+        <s v="VL_IGC"/>
+        <s v="NU_ANO_IGC"/>
+        <s v="DS_REITOR_PRINCIPAL"/>
+        <s v="DS_REPRESENTANTE_LEGAL"/>
+        <s v="DS_SINALIZACAO_VIGENTE"/>
+        <s v="NO_SITUACAO_IES"/>
+        <s v="DS_ENDEREÇO" u="1"/>
+        <s v="DS_ENDERECO_IES" u="1"/>
+        <s v="DS_NUMERO_ENDERECO_IES" u="1"/>
+        <s v="DS_COMPLEMENTO_ENDERECO_IES" u="1"/>
+        <s v="NO_BAIRRO_IES" u="1"/>
+        <s v="NU_CEP_IES" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="TABELA" numFmtId="0">
+      <sharedItems count="2">
+        <s v="ODS_IES"/>
+        <s v="STG_IES"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="45">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="32"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="33"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="34"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="35"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="36"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="37"/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CDD1C3-16F7-45D5-8DDE-1EBD81EB33AC}" name="Tabela dinâmica1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" dataField="1" showAll="0" sortType="ascending">
+      <items count="45">
+        <item x="18"/>
+        <item x="0"/>
+        <item x="8"/>
+        <item x="4"/>
+        <item x="11"/>
+        <item m="1" x="41"/>
+        <item x="22"/>
+        <item x="9"/>
+        <item m="1" x="38"/>
+        <item m="1" x="39"/>
+        <item x="10"/>
+        <item m="1" x="40"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="21"/>
+        <item x="20"/>
+        <item x="27"/>
+        <item x="5"/>
+        <item x="12"/>
+        <item m="1" x="42"/>
+        <item x="14"/>
+        <item x="1"/>
+        <item x="17"/>
+        <item x="23"/>
+        <item x="19"/>
+        <item x="15"/>
+        <item x="26"/>
+        <item x="37"/>
+        <item x="25"/>
+        <item x="3"/>
+        <item x="29"/>
+        <item x="31"/>
+        <item x="33"/>
+        <item x="13"/>
+        <item m="1" x="43"/>
+        <item x="28"/>
+        <item x="2"/>
+        <item x="24"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="16"/>
+        <item x="30"/>
+        <item x="32"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="39">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Contagem de COLUNA" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="7">
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="22">
+            <x v="0"/>
+            <x v="6"/>
+            <x v="8"/>
+            <x v="12"/>
+            <x v="13"/>
+            <x v="14"/>
+            <x v="15"/>
+            <x v="16"/>
+            <x v="17"/>
+            <x v="23"/>
+            <x v="24"/>
+            <x v="25"/>
+            <x v="27"/>
+            <x v="28"/>
+            <x v="29"/>
+            <x v="31"/>
+            <x v="32"/>
+            <x v="33"/>
+            <x v="36"/>
+            <x v="38"/>
+            <x v="42"/>
+            <x v="43"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="35"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="11"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="2">
+            <x v="3"/>
+            <x v="30"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="7">
+            <x v="5"/>
+            <x v="9"/>
+            <x v="18"/>
+            <x v="20"/>
+            <x v="39"/>
+            <x v="40"/>
+            <x v="41"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="19"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="34"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2872,8 +3667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B47513F-EBC0-402E-887C-E14CDBFC32A7}">
   <dimension ref="A1:W202"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.296875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2891,59 +3686,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="120" t="s">
+      <c r="D1" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="120" t="s">
+      <c r="E1" s="112" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="112" t="s">
+      <c r="F1" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="112" t="s">
+      <c r="G1" s="115" t="s">
         <v>616</v>
       </c>
-      <c r="H1" s="114" t="s">
+      <c r="H1" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="116" t="s">
+      <c r="I1" s="120" t="s">
         <v>176</v>
       </c>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="118"/>
-      <c r="V1" s="112" t="s">
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="121"/>
+      <c r="P1" s="121"/>
+      <c r="Q1" s="121"/>
+      <c r="R1" s="121"/>
+      <c r="S1" s="121"/>
+      <c r="T1" s="121"/>
+      <c r="U1" s="122"/>
+      <c r="V1" s="115" t="s">
         <v>7</v>
       </c>
       <c r="W1" s="49"/>
     </row>
     <row r="2" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="119"/>
-      <c r="B2" s="121"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="115"/>
+      <c r="A2" s="113"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="119"/>
       <c r="I2" s="20" t="s">
         <v>8</v>
       </c>
@@ -2983,7 +3778,7 @@
       <c r="U2" s="20" t="s">
         <v>614</v>
       </c>
-      <c r="V2" s="119"/>
+      <c r="V2" s="113"/>
       <c r="W2" s="49"/>
     </row>
     <row r="3" spans="1:23" s="56" customFormat="1" x14ac:dyDescent="0.25">
@@ -15158,16 +15953,16 @@
     <filterColumn colId="19" showButton="0"/>
   </autoFilter>
   <mergeCells count="10">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:U1"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:U1"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15179,10 +15974,10 @@
   <dimension ref="A1:Z83"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="66.69921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15221,21 +16016,21 @@
       <c r="G1" s="123" t="s">
         <v>616</v>
       </c>
-      <c r="H1" s="116" t="s">
+      <c r="H1" s="120" t="s">
         <v>176</v>
       </c>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="118"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="121"/>
+      <c r="P1" s="121"/>
+      <c r="Q1" s="121"/>
+      <c r="R1" s="121"/>
+      <c r="S1" s="121"/>
+      <c r="T1" s="122"/>
       <c r="U1" s="123" t="s">
         <v>7</v>
       </c>
@@ -20764,55 +21559,55 @@
       <c r="W5" s="47"/>
     </row>
     <row r="6" spans="1:23" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="120" t="s">
+      <c r="A6" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="120" t="s">
+      <c r="B6" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="112" t="s">
+      <c r="C6" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="120" t="s">
+      <c r="D6" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="120" t="s">
+      <c r="E6" s="112" t="s">
         <v>185</v>
       </c>
-      <c r="F6" s="112" t="s">
+      <c r="F6" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="114" t="s">
+      <c r="G6" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="116" t="s">
+      <c r="H6" s="120" t="s">
         <v>176</v>
       </c>
-      <c r="I6" s="117"/>
-      <c r="J6" s="117"/>
-      <c r="K6" s="117"/>
-      <c r="L6" s="117"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
-      <c r="Q6" s="117"/>
-      <c r="R6" s="117"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="118"/>
-      <c r="U6" s="112" t="s">
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="121"/>
+      <c r="R6" s="121"/>
+      <c r="S6" s="121"/>
+      <c r="T6" s="122"/>
+      <c r="U6" s="115" t="s">
         <v>7</v>
       </c>
       <c r="V6" s="49"/>
     </row>
     <row r="7" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="119"/>
-      <c r="B7" s="121"/>
-      <c r="C7" s="122"/>
-      <c r="D7" s="121"/>
-      <c r="E7" s="121"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="115"/>
+      <c r="A7" s="113"/>
+      <c r="B7" s="114"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="117"/>
+      <c r="G7" s="119"/>
       <c r="H7" s="20" t="s">
         <v>8</v>
       </c>
@@ -20852,7 +21647,7 @@
       <c r="T7" s="20" t="s">
         <v>614</v>
       </c>
-      <c r="U7" s="119"/>
+      <c r="U7" s="113"/>
       <c r="V7" s="49"/>
     </row>
     <row r="8" spans="1:23" s="48" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -32860,7 +33655,7 @@
       <pane xSplit="2" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -33025,42 +33820,42 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="114" t="s">
+      <c r="A6" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="114" t="s">
+      <c r="B6" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="114" t="s">
+      <c r="C6" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="114" t="s">
+      <c r="D6" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="114" t="s">
+      <c r="E6" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="F6" s="114" t="s">
+      <c r="F6" s="118" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="114" t="s">
+      <c r="G6" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="116" t="s">
+      <c r="H6" s="120" t="s">
         <v>176</v>
       </c>
-      <c r="I6" s="117"/>
-      <c r="J6" s="117"/>
-      <c r="K6" s="117"/>
-      <c r="L6" s="117"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
-      <c r="Q6" s="117"/>
-      <c r="R6" s="117"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="118"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="121"/>
+      <c r="R6" s="121"/>
+      <c r="S6" s="121"/>
+      <c r="T6" s="122"/>
       <c r="U6" s="123" t="s">
         <v>7</v>
       </c>
@@ -33071,13 +33866,13 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="133"/>
-      <c r="B7" s="133"/>
-      <c r="C7" s="133"/>
-      <c r="D7" s="133"/>
-      <c r="E7" s="133"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="133"/>
+      <c r="A7" s="131"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="131"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="133"/>
+      <c r="G7" s="131"/>
       <c r="H7" s="6" t="s">
         <v>8</v>
       </c>
@@ -33220,26 +34015,26 @@
       <c r="A10" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="131"/>
-      <c r="C10" s="131"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="131"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="131"/>
-      <c r="H10" s="131"/>
-      <c r="I10" s="131"/>
-      <c r="J10" s="131"/>
-      <c r="K10" s="131"/>
-      <c r="L10" s="131"/>
-      <c r="M10" s="131"/>
-      <c r="N10" s="131"/>
-      <c r="O10" s="131"/>
-      <c r="P10" s="131"/>
-      <c r="Q10" s="131"/>
-      <c r="R10" s="131"/>
-      <c r="S10" s="131"/>
-      <c r="T10" s="131"/>
-      <c r="U10" s="131"/>
+      <c r="B10" s="132"/>
+      <c r="C10" s="132"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="132"/>
+      <c r="H10" s="132"/>
+      <c r="I10" s="132"/>
+      <c r="J10" s="132"/>
+      <c r="K10" s="132"/>
+      <c r="L10" s="132"/>
+      <c r="M10" s="132"/>
+      <c r="N10" s="132"/>
+      <c r="O10" s="132"/>
+      <c r="P10" s="132"/>
+      <c r="Q10" s="132"/>
+      <c r="R10" s="132"/>
+      <c r="S10" s="132"/>
+      <c r="T10" s="132"/>
+      <c r="U10" s="132"/>
       <c r="V10" s="8"/>
       <c r="W10" s="8"/>
       <c r="X10" s="8"/>
@@ -36430,26 +37225,26 @@
       <c r="A60" s="126" t="s">
         <v>111</v>
       </c>
-      <c r="B60" s="131"/>
-      <c r="C60" s="131"/>
-      <c r="D60" s="131"/>
-      <c r="E60" s="131"/>
-      <c r="F60" s="131"/>
-      <c r="G60" s="131"/>
-      <c r="H60" s="131"/>
-      <c r="I60" s="131"/>
-      <c r="J60" s="131"/>
-      <c r="K60" s="131"/>
-      <c r="L60" s="131"/>
-      <c r="M60" s="131"/>
-      <c r="N60" s="131"/>
-      <c r="O60" s="131"/>
-      <c r="P60" s="131"/>
-      <c r="Q60" s="131"/>
-      <c r="R60" s="131"/>
-      <c r="S60" s="131"/>
-      <c r="T60" s="131"/>
-      <c r="U60" s="131"/>
+      <c r="B60" s="132"/>
+      <c r="C60" s="132"/>
+      <c r="D60" s="132"/>
+      <c r="E60" s="132"/>
+      <c r="F60" s="132"/>
+      <c r="G60" s="132"/>
+      <c r="H60" s="132"/>
+      <c r="I60" s="132"/>
+      <c r="J60" s="132"/>
+      <c r="K60" s="132"/>
+      <c r="L60" s="132"/>
+      <c r="M60" s="132"/>
+      <c r="N60" s="132"/>
+      <c r="O60" s="132"/>
+      <c r="P60" s="132"/>
+      <c r="Q60" s="132"/>
+      <c r="R60" s="132"/>
+      <c r="S60" s="132"/>
+      <c r="T60" s="132"/>
+      <c r="U60" s="132"/>
       <c r="V60" s="8"/>
       <c r="W60" s="8"/>
       <c r="X60" s="8"/>
@@ -38443,6 +39238,11 @@
   </sheetData>
   <autoFilter ref="A8:U85" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="12">
+    <mergeCell ref="A10:U10"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="A60:U60"/>
+    <mergeCell ref="H6:T6"/>
     <mergeCell ref="A4:U4"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
@@ -38450,14 +39250,1041 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="A10:U10"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="A60:U60"/>
-    <mergeCell ref="H6:T6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="45" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4091F7-7A9E-41DF-A253-DDCAA2D5CFB0}">
+  <dimension ref="A3:E43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.09765625" style="134" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.09765625" style="134" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="134" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" style="134" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66" style="134" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.796875" style="134"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="137" t="s">
+        <v>652</v>
+      </c>
+      <c r="B3" s="137" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="137" t="s">
+        <v>650</v>
+      </c>
+      <c r="B4" s="134" t="s">
+        <v>649</v>
+      </c>
+      <c r="C4" s="134" t="s">
+        <v>648</v>
+      </c>
+      <c r="D4" s="134" t="s">
+        <v>617</v>
+      </c>
+      <c r="E4" s="134" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="135" t="s">
+        <v>647</v>
+      </c>
+      <c r="B5" s="136"/>
+      <c r="C5" s="134">
+        <v>1</v>
+      </c>
+      <c r="D5" s="134">
+        <v>1</v>
+      </c>
+      <c r="E5" s="134" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="135" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="134">
+        <v>1</v>
+      </c>
+      <c r="C6" s="134">
+        <v>1</v>
+      </c>
+      <c r="D6" s="134">
+        <v>2</v>
+      </c>
+      <c r="E6" s="134" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="135" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="134">
+        <v>1</v>
+      </c>
+      <c r="C7" s="134">
+        <v>1</v>
+      </c>
+      <c r="D7" s="134">
+        <v>2</v>
+      </c>
+      <c r="E7" s="134" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="135" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="134">
+        <v>1</v>
+      </c>
+      <c r="C8" s="136"/>
+      <c r="D8" s="134">
+        <v>1</v>
+      </c>
+      <c r="E8" s="134" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="135" t="s">
+        <v>646</v>
+      </c>
+      <c r="B9" s="134">
+        <v>1</v>
+      </c>
+      <c r="D9" s="134">
+        <v>1</v>
+      </c>
+      <c r="E9" s="134" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="135" t="s">
+        <v>644</v>
+      </c>
+      <c r="B10" s="136"/>
+      <c r="C10" s="134">
+        <v>1</v>
+      </c>
+      <c r="D10" s="134">
+        <v>1</v>
+      </c>
+      <c r="E10" s="134" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="135" t="s">
+        <v>643</v>
+      </c>
+      <c r="B11" s="134">
+        <v>1</v>
+      </c>
+      <c r="C11" s="134">
+        <v>1</v>
+      </c>
+      <c r="D11" s="134">
+        <v>2</v>
+      </c>
+      <c r="E11" s="134" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="135" t="s">
+        <v>642</v>
+      </c>
+      <c r="B12" s="134">
+        <v>1</v>
+      </c>
+      <c r="D12" s="134">
+        <v>1</v>
+      </c>
+      <c r="E12" s="134" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="135" t="s">
+        <v>641</v>
+      </c>
+      <c r="B13" s="136"/>
+      <c r="C13" s="134">
+        <v>1</v>
+      </c>
+      <c r="D13" s="134">
+        <v>1</v>
+      </c>
+      <c r="E13" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="135" t="s">
+        <v>640</v>
+      </c>
+      <c r="B14" s="136"/>
+      <c r="C14" s="134">
+        <v>1</v>
+      </c>
+      <c r="D14" s="134">
+        <v>1</v>
+      </c>
+      <c r="E14" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="135" t="s">
+        <v>639</v>
+      </c>
+      <c r="B15" s="136"/>
+      <c r="C15" s="134">
+        <v>1</v>
+      </c>
+      <c r="D15" s="134">
+        <v>1</v>
+      </c>
+      <c r="E15" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="135" t="s">
+        <v>638</v>
+      </c>
+      <c r="B16" s="136"/>
+      <c r="C16" s="134">
+        <v>1</v>
+      </c>
+      <c r="D16" s="134">
+        <v>1</v>
+      </c>
+      <c r="E16" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="135" t="s">
+        <v>637</v>
+      </c>
+      <c r="B17" s="136"/>
+      <c r="C17" s="134">
+        <v>1</v>
+      </c>
+      <c r="D17" s="134">
+        <v>1</v>
+      </c>
+      <c r="E17" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="135" t="s">
+        <v>636</v>
+      </c>
+      <c r="B18" s="136"/>
+      <c r="C18" s="134">
+        <v>1</v>
+      </c>
+      <c r="D18" s="134">
+        <v>1</v>
+      </c>
+      <c r="E18" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="135" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" s="134">
+        <v>1</v>
+      </c>
+      <c r="C19" s="136"/>
+      <c r="D19" s="134">
+        <v>1</v>
+      </c>
+      <c r="E19" s="134" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="135" t="s">
+        <v>634</v>
+      </c>
+      <c r="B20" s="134">
+        <v>1</v>
+      </c>
+      <c r="C20" s="136"/>
+      <c r="D20" s="134">
+        <v>1</v>
+      </c>
+      <c r="E20" s="134" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="135" t="s">
+        <v>632</v>
+      </c>
+      <c r="B21" s="134">
+        <v>1</v>
+      </c>
+      <c r="C21" s="134">
+        <v>1</v>
+      </c>
+      <c r="D21" s="134">
+        <v>2</v>
+      </c>
+      <c r="E21" s="134" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="135" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="134">
+        <v>1</v>
+      </c>
+      <c r="C22" s="134">
+        <v>1</v>
+      </c>
+      <c r="D22" s="134">
+        <v>2</v>
+      </c>
+      <c r="E22" s="134" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="135" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="136"/>
+      <c r="C23" s="134">
+        <v>1</v>
+      </c>
+      <c r="D23" s="134">
+        <v>1</v>
+      </c>
+      <c r="E23" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="135" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="136"/>
+      <c r="C24" s="134">
+        <v>1</v>
+      </c>
+      <c r="D24" s="134">
+        <v>1</v>
+      </c>
+      <c r="E24" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="135" t="s">
+        <v>631</v>
+      </c>
+      <c r="B25" s="136"/>
+      <c r="C25" s="134">
+        <v>1</v>
+      </c>
+      <c r="D25" s="134">
+        <v>1</v>
+      </c>
+      <c r="E25" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="135" t="s">
+        <v>630</v>
+      </c>
+      <c r="B26" s="134">
+        <v>1</v>
+      </c>
+      <c r="C26" s="134">
+        <v>1</v>
+      </c>
+      <c r="D26" s="134">
+        <v>2</v>
+      </c>
+      <c r="E26" s="134" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="135" t="s">
+        <v>629</v>
+      </c>
+      <c r="B27" s="136"/>
+      <c r="C27" s="134">
+        <v>1</v>
+      </c>
+      <c r="D27" s="134">
+        <v>1</v>
+      </c>
+      <c r="E27" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="135" t="s">
+        <v>627</v>
+      </c>
+      <c r="B28" s="136"/>
+      <c r="C28" s="134">
+        <v>1</v>
+      </c>
+      <c r="D28" s="134">
+        <v>1</v>
+      </c>
+      <c r="E28" s="134" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="135" t="s">
+        <v>625</v>
+      </c>
+      <c r="B29" s="136"/>
+      <c r="C29" s="134">
+        <v>1</v>
+      </c>
+      <c r="D29" s="134">
+        <v>1</v>
+      </c>
+      <c r="E29" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="135" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="134">
+        <v>1</v>
+      </c>
+      <c r="C30" s="136"/>
+      <c r="D30" s="134">
+        <v>1</v>
+      </c>
+      <c r="E30" s="134" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="135" t="s">
+        <v>624</v>
+      </c>
+      <c r="B31" s="136"/>
+      <c r="C31" s="134">
+        <v>1</v>
+      </c>
+      <c r="D31" s="134">
+        <v>1</v>
+      </c>
+      <c r="E31" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="135" t="s">
+        <v>623</v>
+      </c>
+      <c r="B32" s="136"/>
+      <c r="C32" s="134">
+        <v>1</v>
+      </c>
+      <c r="D32" s="134">
+        <v>1</v>
+      </c>
+      <c r="E32" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="135" t="s">
+        <v>622</v>
+      </c>
+      <c r="B33" s="136"/>
+      <c r="C33" s="134">
+        <v>1</v>
+      </c>
+      <c r="D33" s="134">
+        <v>1</v>
+      </c>
+      <c r="E33" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="135" t="s">
+        <v>621</v>
+      </c>
+      <c r="B34" s="134">
+        <v>1</v>
+      </c>
+      <c r="C34" s="136"/>
+      <c r="D34" s="134">
+        <v>1</v>
+      </c>
+      <c r="E34" s="134" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="135" t="s">
+        <v>620</v>
+      </c>
+      <c r="B35" s="136"/>
+      <c r="C35" s="134">
+        <v>1</v>
+      </c>
+      <c r="D35" s="134">
+        <v>1</v>
+      </c>
+      <c r="E35" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="135" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="134">
+        <v>1</v>
+      </c>
+      <c r="C36" s="134">
+        <v>1</v>
+      </c>
+      <c r="D36" s="134">
+        <v>2</v>
+      </c>
+      <c r="E36" s="134" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="135" t="s">
+        <v>167</v>
+      </c>
+      <c r="B37" s="136"/>
+      <c r="C37" s="134">
+        <v>1</v>
+      </c>
+      <c r="D37" s="134">
+        <v>1</v>
+      </c>
+      <c r="E37" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="135" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="134">
+        <v>1</v>
+      </c>
+      <c r="C38" s="136"/>
+      <c r="D38" s="134">
+        <v>1</v>
+      </c>
+      <c r="E38" s="134" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="135" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="134">
+        <v>1</v>
+      </c>
+      <c r="C39" s="136"/>
+      <c r="D39" s="134">
+        <v>1</v>
+      </c>
+      <c r="E39" s="134" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="B40" s="134">
+        <v>1</v>
+      </c>
+      <c r="C40" s="136"/>
+      <c r="D40" s="134">
+        <v>1</v>
+      </c>
+      <c r="E40" s="138" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="135" t="s">
+        <v>619</v>
+      </c>
+      <c r="B41" s="136"/>
+      <c r="C41" s="134">
+        <v>1</v>
+      </c>
+      <c r="D41" s="134">
+        <v>1</v>
+      </c>
+      <c r="E41" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="135" t="s">
+        <v>618</v>
+      </c>
+      <c r="B42" s="136"/>
+      <c r="C42" s="134">
+        <v>1</v>
+      </c>
+      <c r="D42" s="134">
+        <v>1</v>
+      </c>
+      <c r="E42" s="134" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="135" t="s">
+        <v>617</v>
+      </c>
+      <c r="B43" s="134">
+        <v>17</v>
+      </c>
+      <c r="C43" s="134">
+        <v>28</v>
+      </c>
+      <c r="D43" s="134">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC531F11-6FAF-40AB-B475-25F76439BF08}">
+  <dimension ref="A1:B46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.69921875" style="134" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.796875" style="134"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="134" t="s">
+        <v>654</v>
+      </c>
+      <c r="B1" s="134" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="134" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="134" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="134" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="134" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="134" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="134" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="134" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="134" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="134" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="134" t="s">
+        <v>643</v>
+      </c>
+      <c r="B11" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="134" t="s">
+        <v>642</v>
+      </c>
+      <c r="B12" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="134" t="s">
+        <v>646</v>
+      </c>
+      <c r="B13" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="134" t="s">
+        <v>634</v>
+      </c>
+      <c r="B14" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="134" t="s">
+        <v>621</v>
+      </c>
+      <c r="B15" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="134" t="s">
+        <v>632</v>
+      </c>
+      <c r="B16" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="134" t="s">
+        <v>630</v>
+      </c>
+      <c r="B17" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="134" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="134" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="134" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="134" t="s">
+        <v>647</v>
+      </c>
+      <c r="B21" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="134" t="s">
+        <v>631</v>
+      </c>
+      <c r="B22" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="134" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="134" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="134" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="134" t="s">
+        <v>637</v>
+      </c>
+      <c r="B26" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="134" t="s">
+        <v>638</v>
+      </c>
+      <c r="B27" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="134" t="s">
+        <v>644</v>
+      </c>
+      <c r="B28" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="134" t="s">
+        <v>643</v>
+      </c>
+      <c r="B29" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="134" t="s">
+        <v>165</v>
+      </c>
+      <c r="B30" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="134" t="s">
+        <v>167</v>
+      </c>
+      <c r="B31" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="134" t="s">
+        <v>630</v>
+      </c>
+      <c r="B32" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="134" t="s">
+        <v>625</v>
+      </c>
+      <c r="B33" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="134" t="s">
+        <v>629</v>
+      </c>
+      <c r="B34" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="134" t="s">
+        <v>632</v>
+      </c>
+      <c r="B35" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="134" t="s">
+        <v>636</v>
+      </c>
+      <c r="B36" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="134" t="s">
+        <v>620</v>
+      </c>
+      <c r="B37" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="134" t="s">
+        <v>624</v>
+      </c>
+      <c r="B38" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="134" t="s">
+        <v>619</v>
+      </c>
+      <c r="B39" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="134" t="s">
+        <v>623</v>
+      </c>
+      <c r="B40" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="134" t="s">
+        <v>618</v>
+      </c>
+      <c r="B41" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="134" t="s">
+        <v>622</v>
+      </c>
+      <c r="B42" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="134" t="s">
+        <v>641</v>
+      </c>
+      <c r="B43" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="134" t="s">
+        <v>640</v>
+      </c>
+      <c r="B44" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="134" t="s">
+        <v>639</v>
+      </c>
+      <c r="B45" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="134" t="s">
+        <v>627</v>
+      </c>
+      <c r="B46" s="134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B46" xr:uid="{8BF97AB9-69C0-402F-BF7C-BA9CBF873E3D}"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>